<commit_message>
Modify the code to read in .xlsx files using openpyexcel.
</commit_message>
<xml_diff>
--- a/input_files/Resources.xlsx
+++ b/input_files/Resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boama\Desktop\Spring 2021\CS4269\CS4269_Group4_Project\input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\CS_4269_Work\Part1\CS4269_Group4_Project\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D4C41C0-1B48-482D-919B-1A92103A823C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8FEE5B-05A1-4839-9E67-DBB40446B6C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22200" windowHeight="13176" xr2:uid="{0DBEAA4E-5C28-44EC-BEB5-7DE2FDF83393}"/>
+    <workbookView xWindow="3372" yWindow="312" windowWidth="15504" windowHeight="11988" xr2:uid="{0DBEAA4E-5C28-44EC-BEB5-7DE2FDF83393}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Resource</t>
   </si>
@@ -41,62 +41,62 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>analog to population</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>analog to metallic elements</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>analog to timber</t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>analog to metallic alloys</t>
-  </si>
-  <si>
-    <t>R22</t>
-  </si>
-  <si>
-    <t>analog to electronics</t>
-  </si>
-  <si>
-    <t>R23</t>
-  </si>
-  <si>
-    <t>analog to housing (and housing sufficiency)</t>
-  </si>
-  <si>
-    <t>R21'</t>
-  </si>
-  <si>
-    <t>waste</t>
-  </si>
-  <si>
-    <t>R22'</t>
-  </si>
-  <si>
-    <t>R23'</t>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Scaling</t>
+  </si>
+  <si>
+    <t>Threshold1</t>
+  </si>
+  <si>
+    <t>Threshold2</t>
+  </si>
+  <si>
+    <t>rawMaterialModel</t>
+  </si>
+  <si>
+    <t>producedMaterialModel</t>
+  </si>
+  <si>
+    <t>wasteModel</t>
+  </si>
+  <si>
+    <t>metalAlloysWaste</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>metalElements</t>
+  </si>
+  <si>
+    <t>timber</t>
+  </si>
+  <si>
+    <t>metalAlloys</t>
+  </si>
+  <si>
+    <t>electronics</t>
+  </si>
+  <si>
+    <t>housing</t>
+  </si>
+  <si>
+    <t>landArea</t>
+  </si>
+  <si>
+    <t>housingWaste</t>
+  </si>
+  <si>
+    <t>electronicsWaste</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -104,13 +104,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -125,14 +137,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,128 +460,224 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68CBEA8-BFEF-41B1-9520-7DEA93E453FB}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.19921875" style="2"/>
+    <col min="1" max="1" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
-        <v>0</v>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2">
+        <v>50</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2">
         <v>0.8</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="E10" s="2">
+        <v>50</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="E11" s="2">
+        <v>50</v>
+      </c>
+      <c r="F11" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished successor function for TRANSFORM
</commit_message>
<xml_diff>
--- a/input_files/Resources.xlsx
+++ b/input_files/Resources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\CS_4269_Work\Part1\CS4269_Group4_Project\input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiezh\CS4269_Group4_Project\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8FEE5B-05A1-4839-9E67-DBB40446B6C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3C49F2-542A-4232-BDAC-2728BA24BC9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3372" yWindow="312" windowWidth="15504" windowHeight="11988" xr2:uid="{0DBEAA4E-5C28-44EC-BEB5-7DE2FDF83393}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DBEAA4E-5C28-44EC-BEB5-7DE2FDF83393}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Resource</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>electronicsWaste</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>foodWaste</t>
   </si>
 </sst>
 </file>
@@ -460,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68CBEA8-BFEF-41B1-9520-7DEA93E453FB}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -624,25 +630,25 @@
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2">
-        <v>0.8</v>
+        <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="2">
-        <v>50</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="F9" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2">
         <v>0.8</v>
@@ -658,12 +664,12 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2">
-        <v>8</v>
+        <v>0.8</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>8</v>
@@ -674,7 +680,42 @@
       <c r="E11" s="2">
         <v>50</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="2">
+        <v>50</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="2">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
finished part of successor function
</commit_message>
<xml_diff>
--- a/input_files/Resources.xlsx
+++ b/input_files/Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiezh\CS4269_Group4_Project\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3C49F2-542A-4232-BDAC-2728BA24BC9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78733438-DCAF-40EA-A84A-EC4113C593D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DBEAA4E-5C28-44EC-BEB5-7DE2FDF83393}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Resource</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>foodWaste</t>
+  </si>
+  <si>
+    <t>water</t>
   </si>
 </sst>
 </file>
@@ -466,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68CBEA8-BFEF-41B1-9520-7DEA93E453FB}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -574,13 +577,13 @@
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2">
@@ -592,7 +595,7 @@
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
@@ -610,7 +613,7 @@
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
         <v>5</v>
@@ -618,9 +621,7 @@
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2">
         <v>10</v>
       </c>
@@ -630,15 +631,17 @@
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E9" s="2">
         <v>10</v>
       </c>
@@ -648,25 +651,25 @@
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2">
-        <v>0.8</v>
+        <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2">
-        <v>50</v>
-      </c>
-      <c r="F10" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="F10" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>0.8</v>
@@ -682,12 +685,12 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2">
-        <v>8</v>
+        <v>0.8</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>8</v>
@@ -698,11 +701,11 @@
       <c r="E12" s="2">
         <v>50</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2">
         <v>8</v>
@@ -716,6 +719,25 @@
       <c r="E13" s="2">
         <v>50</v>
       </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="2">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="2">
+        <v>50</v>
+      </c>
+      <c r="F14" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
define thresholds and correct mistakes in weights
</commit_message>
<xml_diff>
--- a/input_files/Resources.xlsx
+++ b/input_files/Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiezh\CS4269_Group4_Project\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92683DF-8C66-4895-9F15-AFA879E57E5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063332BE-EB77-44A3-812E-E54B791BC157}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DBEAA4E-5C28-44EC-BEB5-7DE2FDF83393}"/>
   </bookViews>
@@ -513,10 +513,10 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
-        <v>10</v>
+        <v>12000</v>
       </c>
       <c r="F2" s="2">
-        <v>100</v>
+        <v>18000</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -533,10 +533,10 @@
         <v>10</v>
       </c>
       <c r="E3" s="2">
-        <v>10</v>
+        <v>1200</v>
       </c>
       <c r="F3" s="2">
-        <v>100</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -551,10 +551,10 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
-        <v>10</v>
+        <v>8250</v>
       </c>
       <c r="F4" s="2">
-        <v>100</v>
+        <v>27000</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -569,10 +569,10 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2">
-        <v>10</v>
+        <v>15000</v>
       </c>
       <c r="F5" s="2">
-        <v>100</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -580,17 +580,17 @@
         <v>21</v>
       </c>
       <c r="B6" s="2">
-        <v>4300</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2">
-        <v>10</v>
+        <v>40000</v>
       </c>
       <c r="F6" s="2">
-        <v>100</v>
+        <v>55000</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -605,10 +605,10 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2">
-        <v>10</v>
+        <v>700</v>
       </c>
       <c r="F7" s="2">
-        <v>100</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -616,17 +616,17 @@
         <v>14</v>
       </c>
       <c r="B8" s="2">
-        <v>1000</v>
+        <v>4300</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2">
-        <v>10</v>
+        <v>700</v>
       </c>
       <c r="F8" s="2">
-        <v>100</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -643,10 +643,10 @@
         <v>10</v>
       </c>
       <c r="E9" s="2">
-        <v>10</v>
+        <v>14000</v>
       </c>
       <c r="F9" s="2">
-        <v>100</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -661,10 +661,10 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2">
-        <v>10</v>
+        <v>14000</v>
       </c>
       <c r="F10" s="2">
-        <v>100</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -681,7 +681,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="2">
-        <v>50</v>
+        <v>1500</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -699,7 +699,7 @@
         <v>16</v>
       </c>
       <c r="E12" s="2">
-        <v>50</v>
+        <v>1500</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -717,7 +717,7 @@
         <v>16</v>
       </c>
       <c r="E13" s="2">
-        <v>50</v>
+        <v>1500</v>
       </c>
       <c r="F13" s="3"/>
     </row>
@@ -735,7 +735,7 @@
         <v>16</v>
       </c>
       <c r="E14" s="2">
-        <v>50</v>
+        <v>1500</v>
       </c>
       <c r="F14" s="3"/>
     </row>

</xml_diff>